<commit_message>
complete assignment 2 for production mod
</commit_message>
<xml_diff>
--- a/02_activities/assignments/assignment_2_rubric_clean.xlsx
+++ b/02_activities/assignments/assignment_2_rubric_clean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCalderon\projects\dsi_solutions\solutions\production\assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14babe2585354311/Desktop/le files/DSI/module_6_dsi_production/production/02_activities/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A8CED2-F4A6-4E77-9448-0CFD27A9D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{C0852342-B4DD-4AAD-9E9C-10BBBB4B271E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0852342-B4DD-4AAD-9E9C-10BBBB4B271E}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -575,31 +575,31 @@
   <dimension ref="A2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.796875" customWidth="1"/>
-    <col min="4" max="12" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" customWidth="1"/>
+    <col min="4" max="12" width="5.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="52.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -635,7 +635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
@@ -653,7 +653,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="12" t="s">
         <v>20</v>
@@ -669,7 +669,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="12"/>
       <c r="C9" s="5"/>
@@ -683,7 +683,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" s="8" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" s="8" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
@@ -701,7 +701,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
         <v>22</v>
@@ -717,7 +717,7 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
         <v>23</v>
@@ -733,7 +733,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
         <v>24</v>
@@ -749,7 +749,7 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>7</v>
       </c>
@@ -767,7 +767,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>26</v>
@@ -783,7 +783,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>33</v>
@@ -799,7 +799,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>8</v>
       </c>
@@ -817,7 +817,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:12" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="14" t="s">
         <v>27</v>
@@ -833,7 +833,7 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:12" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="14" t="s">
         <v>28</v>
@@ -849,7 +849,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:12" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" s="16" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
         <v>29</v>
@@ -865,7 +865,7 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
     </row>
-    <row r="21" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>32</v>
@@ -899,7 +899,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <f>COUNTA(B7:B22)</f>
         <v>15</v>
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>2</v>
       </c>

</xml_diff>